<commit_message>
📈 Created 'Metting' and 'Request' activity diagrams
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8EA29-3F64-4F7A-ACDA-4F14F8010C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFD65FA-CFF5-43FD-A7A9-003C8B376B08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Git Repo</t>
+  </si>
+  <si>
+    <t>Created 'Metting' and 'Request' activity diagrams</t>
+  </si>
+  <si>
+    <t>Diagrams</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -530,7 +536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="12.75">
       <c r="A2" s="5">
         <v>44230</v>
       </c>
@@ -544,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="12.75">
       <c r="A3" s="9">
         <v>44231</v>
       </c>
@@ -556,7 +562,7 @@
       </c>
       <c r="D3" s="36"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="12.75">
       <c r="A4" s="10">
         <v>44239</v>
       </c>
@@ -570,7 +576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="12.75">
       <c r="A5" s="5">
         <v>44240</v>
       </c>
@@ -584,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="12.75">
       <c r="A6" s="10">
         <v>44240</v>
       </c>
@@ -598,7 +604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="12.75">
       <c r="A7" s="10">
         <v>44242</v>
       </c>
@@ -610,7 +616,7 @@
       </c>
       <c r="D7" s="36"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="10">
         <v>44242</v>
       </c>
@@ -622,7 +628,7 @@
       </c>
       <c r="D8" s="36"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="17">
         <v>44244</v>
       </c>
@@ -634,7 +640,7 @@
       </c>
       <c r="D9" s="36"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="17">
         <v>44244</v>
       </c>
@@ -675,150 +681,158 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="A13" s="27">
+        <v>44252</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12.75">
       <c r="A14" s="23"/>
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="27"/>
       <c r="B15" s="28"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
       <c r="D16" s="26"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
       <c r="C17" s="29"/>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="12.75">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
       <c r="D18" s="26"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="12.75">
       <c r="A19" s="27"/>
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
       <c r="D19" s="30"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="23"/>
       <c r="B20" s="24"/>
       <c r="C20" s="25"/>
       <c r="D20" s="26"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="27"/>
       <c r="B21" s="28"/>
       <c r="C21" s="29"/>
       <c r="D21" s="30"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="12.75">
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="12.75">
       <c r="A23" s="27"/>
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
       <c r="D23" s="30"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="12.75">
       <c r="A24" s="23"/>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
       <c r="D24" s="26"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="12.75">
       <c r="A25" s="27"/>
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
       <c r="D25" s="30"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="12.75">
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
       <c r="D26" s="26"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="12.75">
       <c r="A27" s="27"/>
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
       <c r="D27" s="30"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="12.75">
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
       <c r="D28" s="26"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="12.75">
       <c r="A29" s="27"/>
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
       <c r="D29" s="30"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="12.75">
       <c r="A30" s="23"/>
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="12.75">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="33"/>
       <c r="D31" s="34"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="12.75">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="33"/>
       <c r="D32" s="34"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="31"/>
       <c r="B33" s="32"/>
       <c r="C33" s="33"/>
       <c r="D33" s="34"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="12.75">
       <c r="A34" s="31"/>
       <c r="B34" s="32"/>
       <c r="C34" s="33"/>
       <c r="D34" s="34"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="31"/>
       <c r="B35" s="32"/>
       <c r="C35" s="33"/>
       <c r="D35" s="34"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="12.75">
       <c r="A36" s="31"/>
       <c r="B36" s="32"/>
       <c r="C36" s="33"/>
       <c r="D36" s="34"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="12.75">
       <c r="A37" s="31"/>
       <c r="B37" s="32"/>
       <c r="C37" s="33"/>

</xml_diff>

<commit_message>
📝 Wrote the bussniss processes
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFD65FA-CFF5-43FD-A7A9-003C8B376B08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD530AD-80FF-45DF-A47C-7BD800A535ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -85,7 +85,10 @@
     <t>Created 'Metting' and 'Request' activity diagrams</t>
   </si>
   <si>
-    <t>Diagrams</t>
+    <t>Wrote the bussniss processes</t>
+  </si>
+  <si>
+    <t>Domain modelling</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,6 +291,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,10 +514,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -519,7 +525,7 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="86.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
@@ -690,117 +696,123 @@
       <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12.75">
+      <c r="A14" s="27">
+        <v>44252</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0.94236111111111109</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="12.75">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:4" ht="12.75">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:4" ht="12.75">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
     </row>
     <row r="20" spans="1:4" ht="12.75">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
     </row>
     <row r="21" spans="1:4" ht="12.75">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" ht="12.75">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
       <c r="A32" s="31"/>
@@ -6616,10 +6628,17 @@
       <c r="C1000" s="33"/>
       <c r="D1000" s="34"/>
     </row>
+    <row r="1001" spans="1:4" ht="12.75">
+      <c r="A1001" s="31"/>
+      <c r="B1001" s="32"/>
+      <c r="C1001" s="33"/>
+      <c r="D1001" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
📝 Updated busniss processes
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD530AD-80FF-45DF-A47C-7BD800A535ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E05974E-55F6-413C-8269-415B631B9648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Domain modelling</t>
+  </si>
+  <si>
+    <t>Updated busniss processes</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1001"/>
+  <dimension ref="A1:D1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -713,112 +716,118 @@
       <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
+      <c r="A15" s="27">
+        <v>44252</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0.96319444444444446</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="30"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
     </row>
     <row r="18" spans="1:4" ht="12.75">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:4" ht="12.75">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
     </row>
     <row r="20" spans="1:4" ht="12.75">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" ht="12.75">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
     </row>
     <row r="22" spans="1:4" ht="12.75">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="31"/>
@@ -6634,11 +6643,17 @@
       <c r="C1001" s="33"/>
       <c r="D1001" s="34"/>
     </row>
+    <row r="1002" spans="1:4" ht="12.75">
+      <c r="A1002" s="31"/>
+      <c r="B1002" s="32"/>
+      <c r="C1002" s="33"/>
+      <c r="D1002" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D13:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
📝 Update use cases Grouped edit and remove post
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F0F59A-32A0-486C-8BA8-F75A65CD42A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCBCAB7-D614-4BD4-9626-F291E33DA4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13485" yWindow="6345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5910" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Wrote first 7 use cases details</t>
+  </si>
+  <si>
+    <t>Updated use cases - Grouped edit and remove post</t>
   </si>
 </sst>
 </file>
@@ -303,6 +306,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -313,10 +320,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +538,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1006"/>
+  <dimension ref="A1:D1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -573,7 +576,7 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -587,7 +590,7 @@
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="12.75">
       <c r="A4" s="10">
@@ -627,7 +630,7 @@
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="39" t="s">
         <v>12</v>
       </c>
     </row>
@@ -641,7 +644,7 @@
       <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="10">
@@ -653,7 +656,7 @@
       <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="38"/>
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="17">
@@ -665,7 +668,7 @@
       <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="17">
@@ -677,7 +680,7 @@
       <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="19">
@@ -717,7 +720,7 @@
       <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="40" t="s">
         <v>22</v>
       </c>
     </row>
@@ -731,7 +734,7 @@
       <c r="C14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="27">
@@ -740,10 +743,10 @@
       <c r="B15" s="28">
         <v>0.96319444444444446</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="27">
@@ -752,10 +755,10 @@
       <c r="B16" s="28">
         <v>0.63194444444444442</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="23">
@@ -767,7 +770,7 @@
       <c r="C17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="35" t="s">
         <v>4</v>
       </c>
     </row>
@@ -778,10 +781,10 @@
       <c r="B18" s="28">
         <v>0.7319444444444444</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="40" t="s">
         <v>22</v>
       </c>
     </row>
@@ -792,10 +795,10 @@
       <c r="B19" s="28">
         <v>0.7319444444444444</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="38"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="27">
@@ -804,10 +807,10 @@
       <c r="B20" s="28">
         <v>0.88680555555555562</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="38"/>
+      <c r="D20" s="40"/>
     </row>
     <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="27">
@@ -816,106 +819,112 @@
       <c r="B21" s="28">
         <v>0.88680555555555562</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="38"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:4" ht="12.75">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="27">
+        <v>44255</v>
+      </c>
+      <c r="B22" s="28">
+        <v>0.62291666666666667</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="40"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="34"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
       <c r="A38" s="31"/>
@@ -6731,12 +6740,18 @@
       <c r="C1006" s="33"/>
       <c r="D1006" s="34"/>
     </row>
+    <row r="1007" spans="1:4" ht="12.75">
+      <c r="A1007" s="31"/>
+      <c r="B1007" s="32"/>
+      <c r="C1007" s="33"/>
+      <c r="D1007" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D18:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📈 Added use cases diagram
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCBCAB7-D614-4BD4-9626-F291E33DA4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0304A65F-9C79-442B-8306-0F2A7BF07896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5910" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Updated use cases - Grouped edit and remove post</t>
+  </si>
+  <si>
+    <t>Created use cases diagram</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1007"/>
+  <dimension ref="A1:D1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -837,100 +840,106 @@
       <c r="D22" s="40"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="27">
+        <v>44255</v>
+      </c>
+      <c r="B23" s="28">
+        <v>0.62638888888888888</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="26"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="34"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
       <c r="A39" s="31"/>
@@ -6746,12 +6755,18 @@
       <c r="C1007" s="33"/>
       <c r="D1007" s="34"/>
     </row>
+    <row r="1008" spans="1:4" ht="12.75">
+      <c r="A1008" s="31"/>
+      <c r="B1008" s="32"/>
+      <c r="C1008" s="33"/>
+      <c r="D1008" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D18:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📈 Created Return-tool activity diagram
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0304A65F-9C79-442B-8306-0F2A7BF07896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B202D4-D43D-4854-9513-ECBC1E8C3520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5910" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Created use cases diagram</t>
+  </si>
+  <si>
+    <t>Created return-tool activity diagram</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1008"/>
+  <dimension ref="A1:D1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -852,100 +855,106 @@
       <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="27">
+        <v>44255</v>
+      </c>
+      <c r="B24" s="28">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="27"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="34"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
     </row>
     <row r="40" spans="1:4" ht="12.75">
       <c r="A40" s="31"/>
@@ -6761,12 +6770,18 @@
       <c r="C1008" s="33"/>
       <c r="D1008" s="34"/>
     </row>
+    <row r="1009" spans="1:4" ht="12.75">
+      <c r="A1009" s="31"/>
+      <c r="B1009" s="32"/>
+      <c r="C1009" s="33"/>
+      <c r="D1009" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="D18:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📝 Update use cases refined them and improved first steps
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B202D4-D43D-4854-9513-ECBC1E8C3520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAB05DE-0A31-4660-A9E7-79E4D1482DA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Created return-tool activity diagram</t>
+  </si>
+  <si>
+    <t>Updated the use cases- refined them and improved the first steps</t>
   </si>
 </sst>
 </file>
@@ -332,6 +335,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC9DAF8"/>
+      <color rgb="FFA4C2F4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -544,10 +553,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1009"/>
+  <dimension ref="A1:D1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -867,100 +876,106 @@
       <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="27">
+        <v>44258</v>
+      </c>
+      <c r="B25" s="28">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="26"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="34"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:4" ht="12.75">
       <c r="A41" s="31"/>
@@ -6776,12 +6791,18 @@
       <c r="C1009" s="33"/>
       <c r="D1009" s="34"/>
     </row>
+    <row r="1010" spans="1:4" ht="12.75">
+      <c r="A1010" s="31"/>
+      <c r="B1010" s="32"/>
+      <c r="C1010" s="33"/>
+      <c r="D1010" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="D18:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📝 Update Log Created the flutter project
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAB05DE-0A31-4660-A9E7-79E4D1482DA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEACDAD4-D4BA-4D93-881A-D9CFDB8168C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Updated the use cases- refined them and improved the first steps</t>
+  </si>
+  <si>
+    <t>Created new flutter project</t>
+  </si>
+  <si>
+    <t>Implementaion</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,7 @@
   <dimension ref="A1:D1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -888,10 +894,18 @@
       <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="23">
+        <v>44259</v>
+      </c>
+      <c r="B26" s="24">
+        <v>0.10347222222222223</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="12.75">
       <c r="A27" s="27"/>

</xml_diff>

<commit_message>
📝 Wrote first 11 FRs
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEACDAD4-D4BA-4D93-881A-D9CFDB8168C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F68184-99E6-4E63-9D6C-C875625523EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Implementaion</t>
+  </si>
+  <si>
+    <t>Wrote first 11 FRs</t>
   </si>
 </sst>
 </file>
@@ -561,8 +564,8 @@
   </sheetPr>
   <dimension ref="A1:D1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -908,10 +911,18 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="27">
+        <v>44259</v>
+      </c>
+      <c r="B27" s="28">
+        <v>0.73402777777777783</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="12.75">
       <c r="A28" s="23"/>

</xml_diff>

<commit_message>
📝 Wrote an extra 12 FRs
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F68184-99E6-4E63-9D6C-C875625523EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8DC077-DAC5-451B-B081-1C799FA437D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Wrote first 11 FRs</t>
+  </si>
+  <si>
+    <t>Wrote an extra 12 FRs</t>
   </si>
 </sst>
 </file>
@@ -562,10 +565,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1010"/>
+  <dimension ref="A1:D1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -920,93 +923,99 @@
       <c r="C27" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="27">
+        <v>44259</v>
+      </c>
+      <c r="B28" s="28">
+        <v>0.96875</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="30"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="27"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
     </row>
     <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" ht="12.75">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="34"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
     </row>
     <row r="42" spans="1:4" ht="12.75">
       <c r="A42" s="31"/>
@@ -6822,12 +6831,19 @@
       <c r="C1010" s="33"/>
       <c r="D1010" s="34"/>
     </row>
+    <row r="1011" spans="1:4" ht="12.75">
+      <c r="A1011" s="31"/>
+      <c r="B1011" s="32"/>
+      <c r="C1011" s="33"/>
+      <c r="D1011" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="D18:D25"/>
+    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📝 Wrote FRs for MSS for UC 5, 6, and 10
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8DC077-DAC5-451B-B081-1C799FA437D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2C2B6D-4B57-434E-A5E4-12E8ABBCCB33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Wrote an extra 12 FRs</t>
+  </si>
+  <si>
+    <t>Wrote 9 FRs for main success scenario for use cases 5, 6, and 10</t>
   </si>
 </sst>
 </file>
@@ -565,10 +568,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1011"/>
+  <dimension ref="A1:D1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -940,88 +943,94 @@
       <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
+      <c r="A29" s="27">
+        <v>44260</v>
+      </c>
+      <c r="B29" s="28">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="26"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:4" ht="12.75">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:4" ht="12.75">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="26"/>
     </row>
     <row r="43" spans="1:4" ht="12.75">
       <c r="A43" s="31"/>
@@ -6836,6 +6845,12 @@
       <c r="B1011" s="32"/>
       <c r="C1011" s="33"/>
       <c r="D1011" s="34"/>
+    </row>
+    <row r="1012" spans="1:4" ht="12.75">
+      <c r="A1012" s="31"/>
+      <c r="B1012" s="32"/>
+      <c r="C1012" s="33"/>
+      <c r="D1012" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6843,7 +6858,7 @@
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="D18:D25"/>
-    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D27:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📝 Wrote extensions for UC1
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2C2B6D-4B57-434E-A5E4-12E8ABBCCB33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C93DC8-9622-4984-A628-8749C3BE07D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Wrote 9 FRs for main success scenario for use cases 5, 6, and 10</t>
+  </si>
+  <si>
+    <t>Wrote extensions for UC1</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <dimension ref="A1:D1012"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -955,10 +958,18 @@
       <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="23">
+        <v>44260</v>
+      </c>
+      <c r="B30" s="24">
+        <v>0.71319444444444446</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="12.75">
       <c r="A31" s="27"/>

</xml_diff>

<commit_message>
📝 Wrote extensions for UC2
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C93DC8-9622-4984-A628-8749C3BE07D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10091CC8-0A57-4D9E-85AA-75E1412F51CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,9 @@
   <si>
     <t>Wrote extensions for UC1</t>
   </si>
+  <si>
+    <t>Wrote extensions for UC2</t>
+  </si>
 </sst>
 </file>
 
@@ -241,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,6 +350,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +575,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1012"/>
+  <dimension ref="A1:D1013"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -972,82 +976,88 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="23">
+        <v>44260</v>
+      </c>
+      <c r="B31" s="24">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="27"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
     </row>
     <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" ht="12.75">
-      <c r="A41" s="27"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
     </row>
     <row r="42" spans="1:4" ht="12.75">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="26"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:4" ht="12.75">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="34"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="26"/>
     </row>
     <row r="44" spans="1:4" ht="12.75">
       <c r="A44" s="31"/>
@@ -6862,6 +6872,12 @@
       <c r="B1012" s="32"/>
       <c r="C1012" s="33"/>
       <c r="D1012" s="34"/>
+    </row>
+    <row r="1013" spans="1:4" ht="12.75">
+      <c r="A1013" s="31"/>
+      <c r="B1013" s="32"/>
+      <c r="C1013" s="33"/>
+      <c r="D1013" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
📝 Wrote extensions for UC3
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10091CC8-0A57-4D9E-85AA-75E1412F51CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80710FD6-3062-40BC-BD83-CFC97CDF0495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Wrote extensions for UC2</t>
+  </si>
+  <si>
+    <t>Wrote extensions for UC3</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1013"/>
+  <dimension ref="A1:D1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -988,15 +991,21 @@
       <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="23">
+        <v>44260</v>
+      </c>
+      <c r="B32" s="24">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="23"/>
       <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
+      <c r="C33" s="41"/>
       <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
@@ -1060,16 +1069,16 @@
       <c r="D43" s="26"/>
     </row>
     <row r="44" spans="1:4" ht="12.75">
-      <c r="A44" s="31"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="34"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:4" ht="12.75">
-      <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="34"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="26"/>
     </row>
     <row r="46" spans="1:4" ht="12.75">
       <c r="A46" s="31"/>
@@ -6878,6 +6887,18 @@
       <c r="B1013" s="32"/>
       <c r="C1013" s="33"/>
       <c r="D1013" s="34"/>
+    </row>
+    <row r="1014" spans="1:4" ht="12.75">
+      <c r="A1014" s="31"/>
+      <c r="B1014" s="32"/>
+      <c r="C1014" s="33"/>
+      <c r="D1014" s="34"/>
+    </row>
+    <row r="1015" spans="1:4" ht="12.75">
+      <c r="A1015" s="31"/>
+      <c r="B1015" s="32"/>
+      <c r="C1015" s="33"/>
+      <c r="D1015" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
📝 Wrote extensions for UC5
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80710FD6-3062-40BC-BD83-CFC97CDF0495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A103D66-6FB3-4BC8-82B3-567E24C261D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Wrote extensions for UC3</t>
+  </si>
+  <si>
+    <t>Wrote extensions for UC5</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
   <dimension ref="A1:D1015"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1003,9 +1006,15 @@
       <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="41"/>
+      <c r="A33" s="23">
+        <v>44260</v>
+      </c>
+      <c r="B33" s="24">
+        <v>0.74791666666666667</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>39</v>
+      </c>
       <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">

</xml_diff>

<commit_message>
📝 Wrote extensions for UC6 and UC8
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A103D66-6FB3-4BC8-82B3-567E24C261D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E760AAA7-88D1-4475-86FB-BFE62DB87172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Wrote extensions for UC5</t>
+  </si>
+  <si>
+    <t>Wrote extensions for UC6</t>
+  </si>
+  <si>
+    <t>Wrote extensions for UC8</t>
   </si>
 </sst>
 </file>
@@ -346,6 +352,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,7 +363,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +587,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1015"/>
+  <dimension ref="A1:D1017"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -619,7 +625,7 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>6</v>
       </c>
     </row>
@@ -633,7 +639,7 @@
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="1:4" ht="12.75">
       <c r="A4" s="10">
@@ -673,7 +679,7 @@
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>12</v>
       </c>
     </row>
@@ -687,7 +693,7 @@
       <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="39"/>
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="10">
@@ -699,7 +705,7 @@
       <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="38"/>
+      <c r="D8" s="39"/>
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="17">
@@ -711,7 +717,7 @@
       <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="39"/>
     </row>
     <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="17">
@@ -723,7 +729,7 @@
       <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="38"/>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="19">
@@ -763,7 +769,7 @@
       <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="41" t="s">
         <v>22</v>
       </c>
     </row>
@@ -777,7 +783,7 @@
       <c r="C14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="27">
@@ -789,7 +795,7 @@
       <c r="C15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="40"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="27">
@@ -801,7 +807,7 @@
       <c r="C16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="40"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="23">
@@ -827,7 +833,7 @@
       <c r="C18" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>22</v>
       </c>
     </row>
@@ -841,7 +847,7 @@
       <c r="C19" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="27">
@@ -853,7 +859,7 @@
       <c r="C20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="27">
@@ -865,7 +871,7 @@
       <c r="C21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="40"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:4" ht="12.75">
       <c r="A22" s="27">
@@ -877,7 +883,7 @@
       <c r="C22" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="40"/>
+      <c r="D22" s="41"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
       <c r="A23" s="27">
@@ -889,7 +895,7 @@
       <c r="C23" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
       <c r="A24" s="27">
@@ -901,7 +907,7 @@
       <c r="C24" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
       <c r="A25" s="27">
@@ -913,7 +919,7 @@
       <c r="C25" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
       <c r="A26" s="23">
@@ -939,7 +945,7 @@
       <c r="C27" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -953,7 +959,7 @@
       <c r="C28" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="40"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
       <c r="A29" s="27">
@@ -965,7 +971,7 @@
       <c r="C29" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="40"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
       <c r="A30" s="23">
@@ -988,7 +994,7 @@
       <c r="B31" s="24">
         <v>0.72013888888888899</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="37" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="26"/>
@@ -1000,7 +1006,7 @@
       <c r="B32" s="24">
         <v>0.73263888888888884</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D32" s="26"/>
@@ -1012,21 +1018,33 @@
       <c r="B33" s="24">
         <v>0.74791666666666667</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="A34" s="23">
+        <v>44262</v>
+      </c>
+      <c r="B34" s="24">
+        <v>0.18402777777777779</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="23">
+        <v>44262</v>
+      </c>
+      <c r="B35" s="24">
+        <v>0.19375000000000001</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>41</v>
+      </c>
       <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
@@ -1090,16 +1108,16 @@
       <c r="D45" s="26"/>
     </row>
     <row r="46" spans="1:4" ht="12.75">
-      <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="34"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:4" ht="12.75">
-      <c r="A47" s="31"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="34"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:4" ht="12.75">
       <c r="A48" s="31"/>
@@ -6908,6 +6926,18 @@
       <c r="B1015" s="32"/>
       <c r="C1015" s="33"/>
       <c r="D1015" s="34"/>
+    </row>
+    <row r="1016" spans="1:4" ht="12.75">
+      <c r="A1016" s="31"/>
+      <c r="B1016" s="32"/>
+      <c r="C1016" s="33"/>
+      <c r="D1016" s="34"/>
+    </row>
+    <row r="1017" spans="1:4" ht="12.75">
+      <c r="A1017" s="31"/>
+      <c r="B1017" s="32"/>
+      <c r="C1017" s="33"/>
+      <c r="D1017" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
📝 Updated UC4 and wrote its extensions
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E760AAA7-88D1-4475-86FB-BFE62DB87172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044A6D1B-ED60-4EBE-84F5-89D9549B66A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,12 @@
   <si>
     <t>Wrote extensions for UC8</t>
   </si>
+  <si>
+    <t>Wrote extensions for UC9, UC10, UC11</t>
+  </si>
+  <si>
+    <t>Updated UC4 and wrote its extensions</t>
+  </si>
 </sst>
 </file>
 
@@ -256,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +367,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -587,10 +596,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1017"/>
+  <dimension ref="A1:D1019"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -983,7 +992,7 @@
       <c r="C30" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="42" t="s">
         <v>22</v>
       </c>
     </row>
@@ -997,7 +1006,7 @@
       <c r="C31" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="42"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
       <c r="A32" s="23">
@@ -1009,7 +1018,7 @@
       <c r="C32" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="42"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="23">
@@ -1021,7 +1030,7 @@
       <c r="C33" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
       <c r="A34" s="23">
@@ -1033,7 +1042,7 @@
       <c r="C34" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="26"/>
+      <c r="D34" s="42"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="23">
@@ -1045,19 +1054,31 @@
       <c r="C35" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
+      <c r="A36" s="23">
+        <v>44263</v>
+      </c>
+      <c r="B36" s="24">
+        <v>0.12361111111111112</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="42"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="23">
+        <v>44263</v>
+      </c>
+      <c r="B37" s="24">
+        <v>0.65625</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="42"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
       <c r="A38" s="27"/>
@@ -1120,16 +1141,16 @@
       <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:4" ht="12.75">
-      <c r="A48" s="31"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="34"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="30"/>
     </row>
     <row r="49" spans="1:4" ht="12.75">
-      <c r="A49" s="31"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="34"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="26"/>
     </row>
     <row r="50" spans="1:4" ht="12.75">
       <c r="A50" s="31"/>
@@ -6939,8 +6960,21 @@
       <c r="C1017" s="33"/>
       <c r="D1017" s="34"/>
     </row>
+    <row r="1018" spans="1:4" ht="12.75">
+      <c r="A1018" s="31"/>
+      <c r="B1018" s="32"/>
+      <c r="C1018" s="33"/>
+      <c r="D1018" s="34"/>
+    </row>
+    <row r="1019" spans="1:4" ht="12.75">
+      <c r="A1019" s="31"/>
+      <c r="B1019" s="32"/>
+      <c r="C1019" s="33"/>
+      <c r="D1019" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="D30:D37"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>

</xml_diff>

<commit_message>
📝 Updated UC7 and wrote its extensions
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044A6D1B-ED60-4EBE-84F5-89D9549B66A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE77954-3A18-4491-865D-8433BA59F2D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Updated UC4 and wrote its extensions</t>
+  </si>
+  <si>
+    <t>Updated UC7 and wrote its extensions</t>
   </si>
 </sst>
 </file>
@@ -359,6 +362,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,9 +373,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,10 +599,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1019"/>
+  <dimension ref="A1:D1020"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -634,7 +637,7 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>6</v>
       </c>
     </row>
@@ -648,7 +651,7 @@
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="12.75">
       <c r="A4" s="10">
@@ -688,7 +691,7 @@
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>12</v>
       </c>
     </row>
@@ -702,7 +705,7 @@
       <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="10">
@@ -714,7 +717,7 @@
       <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="17">
@@ -726,7 +729,7 @@
       <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="17">
@@ -738,7 +741,7 @@
       <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="19">
@@ -778,7 +781,7 @@
       <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="42" t="s">
         <v>22</v>
       </c>
     </row>
@@ -792,7 +795,7 @@
       <c r="C14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="27">
@@ -804,7 +807,7 @@
       <c r="C15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="42"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="27">
@@ -816,7 +819,7 @@
       <c r="C16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="23">
@@ -842,7 +845,7 @@
       <c r="C18" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="42" t="s">
         <v>22</v>
       </c>
     </row>
@@ -856,7 +859,7 @@
       <c r="C19" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="42"/>
     </row>
     <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="27">
@@ -868,7 +871,7 @@
       <c r="C20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="27">
@@ -880,7 +883,7 @@
       <c r="C21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4" ht="12.75">
       <c r="A22" s="27">
@@ -892,7 +895,7 @@
       <c r="C22" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="42"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
       <c r="A23" s="27">
@@ -904,7 +907,7 @@
       <c r="C23" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
       <c r="A24" s="27">
@@ -916,7 +919,7 @@
       <c r="C24" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
       <c r="A25" s="27">
@@ -928,7 +931,7 @@
       <c r="C25" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="42"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
       <c r="A26" s="23">
@@ -954,7 +957,7 @@
       <c r="C27" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="42" t="s">
         <v>9</v>
       </c>
     </row>
@@ -968,7 +971,7 @@
       <c r="C28" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="41"/>
+      <c r="D28" s="42"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
       <c r="A29" s="27">
@@ -980,7 +983,7 @@
       <c r="C29" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="42"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
       <c r="A30" s="23">
@@ -992,7 +995,7 @@
       <c r="C30" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="38" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1006,7 +1009,7 @@
       <c r="C31" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="42"/>
+      <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
       <c r="A32" s="23">
@@ -1018,7 +1021,7 @@
       <c r="C32" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="42"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="23">
@@ -1030,7 +1033,7 @@
       <c r="C33" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="42"/>
+      <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
       <c r="A34" s="23">
@@ -1042,7 +1045,7 @@
       <c r="C34" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="42"/>
+      <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="23">
@@ -1054,7 +1057,7 @@
       <c r="C35" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="42"/>
+      <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
       <c r="A36" s="23">
@@ -1066,7 +1069,7 @@
       <c r="C36" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="42"/>
+      <c r="D36" s="38"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
       <c r="A37" s="23">
@@ -1078,85 +1081,91 @@
       <c r="C37" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="42"/>
+      <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
+      <c r="A38" s="23">
+        <v>44263</v>
+      </c>
+      <c r="B38" s="24">
+        <v>0.87013888888888891</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="38"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:4" ht="12.75">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:4" ht="12.75">
-      <c r="A42" s="27"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="30"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="26"/>
     </row>
     <row r="43" spans="1:4" ht="12.75">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:4" ht="12.75">
-      <c r="A44" s="27"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="30"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
     </row>
     <row r="45" spans="1:4" ht="12.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:4" ht="12.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="30"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="26"/>
     </row>
     <row r="47" spans="1:4" ht="12.75">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:4" ht="12.75">
-      <c r="A48" s="27"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="26"/>
     </row>
     <row r="49" spans="1:4" ht="12.75">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="26"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="30"/>
     </row>
     <row r="50" spans="1:4" ht="12.75">
-      <c r="A50" s="31"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="34"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="1:4" ht="12.75">
       <c r="A51" s="31"/>
@@ -6972,14 +6981,20 @@
       <c r="C1019" s="33"/>
       <c r="D1019" s="34"/>
     </row>
+    <row r="1020" spans="1:4" ht="12.75">
+      <c r="A1020" s="31"/>
+      <c r="B1020" s="32"/>
+      <c r="C1020" s="33"/>
+      <c r="D1020" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="D30:D37"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="D18:D25"/>
     <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📝 Wrote FRs for UC4, UC7, and all UCs extensions.
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE77954-3A18-4491-865D-8433BA59F2D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A374CB8-68B9-433E-8C56-6DB44D8515C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,9 @@
   <si>
     <t>Updated UC7 and wrote its extensions</t>
   </si>
+  <si>
+    <t>Wrote FRs for UC4, UC7, and all UCs extensions.</t>
+  </si>
 </sst>
 </file>
 
@@ -175,6 +178,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -185,10 +189,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -362,9 +368,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,6 +376,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -602,7 +608,7 @@
   <dimension ref="A1:D1020"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -637,7 +643,7 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>6</v>
       </c>
     </row>
@@ -651,7 +657,7 @@
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="1:4" ht="12.75">
       <c r="A4" s="10">
@@ -691,7 +697,7 @@
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>12</v>
       </c>
     </row>
@@ -705,7 +711,7 @@
       <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="39"/>
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="10">
@@ -717,7 +723,7 @@
       <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="40"/>
+      <c r="D8" s="39"/>
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" s="17">
@@ -729,7 +735,7 @@
       <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="40"/>
+      <c r="D9" s="39"/>
     </row>
     <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="17">
@@ -741,7 +747,7 @@
       <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="19">
@@ -781,7 +787,7 @@
       <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>22</v>
       </c>
     </row>
@@ -795,7 +801,7 @@
       <c r="C14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="42"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="27">
@@ -807,7 +813,7 @@
       <c r="C15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="42"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="27">
@@ -819,7 +825,7 @@
       <c r="C16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="42"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="23">
@@ -845,7 +851,7 @@
       <c r="C18" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="41" t="s">
         <v>22</v>
       </c>
     </row>
@@ -859,7 +865,7 @@
       <c r="C19" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="42"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="27">
@@ -871,7 +877,7 @@
       <c r="C20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="42"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="27">
@@ -883,7 +889,7 @@
       <c r="C21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="42"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:4" ht="12.75">
       <c r="A22" s="27">
@@ -895,7 +901,7 @@
       <c r="C22" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="42"/>
+      <c r="D22" s="41"/>
     </row>
     <row r="23" spans="1:4" ht="12.75">
       <c r="A23" s="27">
@@ -907,7 +913,7 @@
       <c r="C23" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="42"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" ht="12.75">
       <c r="A24" s="27">
@@ -919,7 +925,7 @@
       <c r="C24" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="42"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="1:4" ht="12.75">
       <c r="A25" s="27">
@@ -931,7 +937,7 @@
       <c r="C25" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="42"/>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" spans="1:4" ht="12.75">
       <c r="A26" s="23">
@@ -957,7 +963,7 @@
       <c r="C27" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -971,7 +977,7 @@
       <c r="C28" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="42"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
       <c r="A29" s="27">
@@ -983,7 +989,7 @@
       <c r="C29" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:4" ht="12.75">
       <c r="A30" s="23">
@@ -995,7 +1001,7 @@
       <c r="C30" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="42" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1009,7 +1015,7 @@
       <c r="C31" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="38"/>
+      <c r="D31" s="42"/>
     </row>
     <row r="32" spans="1:4" ht="12.75">
       <c r="A32" s="23">
@@ -1021,7 +1027,7 @@
       <c r="C32" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="38"/>
+      <c r="D32" s="42"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="23">
@@ -1033,7 +1039,7 @@
       <c r="C33" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="38"/>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
       <c r="A34" s="23">
@@ -1045,7 +1051,7 @@
       <c r="C34" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="38"/>
+      <c r="D34" s="42"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="23">
@@ -1057,7 +1063,7 @@
       <c r="C35" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="38"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="1:4" ht="12.75">
       <c r="A36" s="23">
@@ -1069,7 +1075,7 @@
       <c r="C36" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="38"/>
+      <c r="D36" s="42"/>
     </row>
     <row r="37" spans="1:4" ht="12.75">
       <c r="A37" s="23">
@@ -1081,7 +1087,7 @@
       <c r="C37" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="38"/>
+      <c r="D37" s="42"/>
     </row>
     <row r="38" spans="1:4" ht="12.75">
       <c r="A38" s="23">
@@ -1093,13 +1099,21 @@
       <c r="C38" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="38"/>
+      <c r="D38" s="42"/>
     </row>
     <row r="39" spans="1:4" ht="12.75">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="27">
+        <v>44264</v>
+      </c>
+      <c r="B39" s="28">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="12.75">
       <c r="A40" s="23"/>
@@ -6989,12 +7003,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D30:D38"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="D18:D25"/>
     <mergeCell ref="D27:D29"/>
-    <mergeCell ref="D30:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>